<commit_message>
Small fixes on circuit schematic
</commit_message>
<xml_diff>
--- a/calculation/TPS62147_calculation.xlsx
+++ b/calculation/TPS62147_calculation.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\On Going Projects\FPGA\FPGA_Pre_Test\calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD76D05A-31FC-4F4F-9093-C9E7AFFECD9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89061CDF-6AF3-404F-88EE-CAF8749F9D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4790" yWindow="650" windowWidth="17500" windowHeight="8250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TPS62147" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="R1R2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -186,10 +186,10 @@
     <numFmt numFmtId="183" formatCode="0.0&quot;mΩ&quot;"/>
     <numFmt numFmtId="184" formatCode="0.00\A"/>
     <numFmt numFmtId="185" formatCode="0.0&quot;μs&quot;"/>
-    <numFmt numFmtId="187" formatCode="0.0&quot;kΩ&quot;"/>
-    <numFmt numFmtId="188" formatCode="0.00&quot;kΩ&quot;"/>
-    <numFmt numFmtId="192" formatCode="0.00&quot;kHz&quot;"/>
-    <numFmt numFmtId="197" formatCode="0.000&quot;uF&quot;"/>
+    <numFmt numFmtId="186" formatCode="0.0&quot;kΩ&quot;"/>
+    <numFmt numFmtId="187" formatCode="0.00&quot;kΩ&quot;"/>
+    <numFmt numFmtId="188" formatCode="0.00&quot;kHz&quot;"/>
+    <numFmt numFmtId="189" formatCode="0.000&quot;uF&quot;"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -470,7 +470,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -479,7 +479,7 @@
     <xf numFmtId="181" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="182" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="185" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="188" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="187" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -493,7 +493,7 @@
     <xf numFmtId="184" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="187" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="186" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -508,80 +508,76 @@
     <xf numFmtId="179" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="192" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="188" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="189" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="181" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="197" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -957,15 +953,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:A3"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection sqref="A1:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="12" width="9.58203125" customWidth="1"/>
     <col min="13" max="13" width="9.58203125" style="9" customWidth="1"/>
-    <col min="14" max="14" width="9.58203125" style="36" customWidth="1"/>
+    <col min="14" max="14" width="9.58203125" customWidth="1"/>
     <col min="15" max="15" width="10.6640625" customWidth="1"/>
     <col min="16" max="16" width="12.08203125" customWidth="1"/>
     <col min="17" max="19" width="9.58203125" customWidth="1"/>
@@ -975,134 +971,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="43" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
-      <c r="S1" s="38"/>
-      <c r="T1" s="38"/>
-      <c r="U1" s="38"/>
-      <c r="V1" s="38"/>
-      <c r="W1" s="38"/>
-      <c r="X1" s="39"/>
-      <c r="Y1" s="21" t="s">
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21" t="s">
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="21"/>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="21"/>
-      <c r="AG1" s="22"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="36"/>
+      <c r="AG1" s="37"/>
     </row>
     <row r="2" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="23"/>
-      <c r="B2" s="24" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24" t="s">
+      <c r="C2" s="34"/>
+      <c r="D2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24" t="s">
+      <c r="F2" s="34"/>
+      <c r="G2" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="34" t="s">
+      <c r="H2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="34" t="s">
+      <c r="K2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="34" t="s">
+      <c r="L2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="M2" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="41" t="s">
+      <c r="N2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="O2" s="23" t="s">
+      <c r="O2" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="24" t="s">
+      <c r="P2" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="34" t="s">
+      <c r="Q2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="31" t="s">
+      <c r="R2" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="S2" s="31"/>
-      <c r="T2" s="24" t="s">
+      <c r="S2" s="40"/>
+      <c r="T2" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="U2" s="24" t="s">
+      <c r="U2" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="V2" s="24" t="s">
+      <c r="V2" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="24" t="s">
+      <c r="W2" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="24" t="s">
+      <c r="X2" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="24" t="s">
+      <c r="Y2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="24" t="s">
+      <c r="Z2" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="AA2" s="24"/>
-      <c r="AB2" s="24" t="s">
+      <c r="AA2" s="34"/>
+      <c r="AB2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="AC2" s="24" t="s">
+      <c r="AC2" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="AD2" s="24"/>
-      <c r="AE2" s="24" t="s">
+      <c r="AD2" s="34"/>
+      <c r="AE2" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="AF2" s="24"/>
-      <c r="AG2" s="32" t="s">
+      <c r="AF2" s="34"/>
+      <c r="AG2" s="38" t="s">
         <v>29</v>
       </c>
       <c r="AH2" s="10"/>
@@ -1111,66 +1107,66 @@
       <c r="AN2" s="1"/>
       <c r="AQ2" s="1"/>
     </row>
-    <row r="3" spans="1:43" s="36" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="26"/>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="27" t="s">
+      <c r="D3" s="35"/>
+      <c r="E3" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="42"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="43"/>
       <c r="O3" s="26"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="35"/>
-      <c r="R3" s="27" t="s">
+      <c r="P3" s="35"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="S3" s="27" t="s">
+      <c r="S3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="T3" s="28"/>
-      <c r="U3" s="28"/>
-      <c r="V3" s="28"/>
-      <c r="W3" s="28"/>
-      <c r="X3" s="28"/>
-      <c r="Y3" s="28"/>
-      <c r="Z3" s="27" t="s">
+      <c r="T3" s="35"/>
+      <c r="U3" s="35"/>
+      <c r="V3" s="35"/>
+      <c r="W3" s="35"/>
+      <c r="X3" s="35"/>
+      <c r="Y3" s="35"/>
+      <c r="Z3" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="AA3" s="27" t="s">
+      <c r="AA3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="AB3" s="28"/>
-      <c r="AC3" s="27" t="s">
+      <c r="AB3" s="35"/>
+      <c r="AC3" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="AD3" s="27" t="s">
+      <c r="AD3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="AE3" s="27" t="s">
+      <c r="AE3" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="AF3" s="27" t="s">
+      <c r="AF3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="AG3" s="29"/>
-      <c r="AH3" s="45"/>
-      <c r="AI3" s="45"/>
+      <c r="AG3" s="39"/>
+      <c r="AH3" s="11"/>
+      <c r="AI3" s="11"/>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A4" s="10">
@@ -1209,10 +1205,10 @@
       <c r="L4" s="18">
         <v>100</v>
       </c>
-      <c r="M4" s="44">
+      <c r="M4" s="23">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="N4" s="37">
+      <c r="N4" s="22">
         <f>IF(G4="LOW",1.25,2.5)</f>
         <v>1.25</v>
       </c>
@@ -1288,7 +1284,7 @@
         <f>IF(G4="LOW",200,100)*C4*10^(-9)/(I4*10^(-6))</f>
         <v>1.2727272727272727</v>
       </c>
-      <c r="AG4" s="33">
+      <c r="AG4" s="21">
         <f>T4/2</f>
         <v>0.79545454545454553</v>
       </c>
@@ -1330,10 +1326,10 @@
       <c r="L5" s="18">
         <v>100</v>
       </c>
-      <c r="M5" s="44">
+      <c r="M5" s="23">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="N5" s="37">
+      <c r="N5" s="22">
         <f>IF(G5="LOW",1.25,2.5)</f>
         <v>1.25</v>
       </c>
@@ -1409,7 +1405,7 @@
         <f>IF(G5="LOW",200,100)*C5*10^(-9)/(I5*10^(-6))</f>
         <v>1.2727272727272727</v>
       </c>
-      <c r="AG5" s="33">
+      <c r="AG5" s="21">
         <f>T5/2</f>
         <v>0.79545454545454553</v>
       </c>
@@ -1451,10 +1447,10 @@
       <c r="L6" s="18">
         <v>100</v>
       </c>
-      <c r="M6" s="44">
+      <c r="M6" s="23">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="N6" s="37">
+      <c r="N6" s="22">
         <f>IF(G6="LOW",1.25,2.5)</f>
         <v>1.25</v>
       </c>
@@ -1530,7 +1526,7 @@
         <f>IF(G6="LOW",200,100)*C6*10^(-9)/(I6*10^(-6))</f>
         <v>1.2727272727272727</v>
       </c>
-      <c r="AG6" s="33">
+      <c r="AG6" s="21">
         <f>T6/2</f>
         <v>0.79545454545454553</v>
       </c>
@@ -1572,10 +1568,10 @@
       <c r="L7" s="18">
         <v>100</v>
       </c>
-      <c r="M7" s="44">
+      <c r="M7" s="23">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="N7" s="37">
+      <c r="N7" s="22">
         <f>IF(G7="LOW",1.25,2.5)</f>
         <v>1.25</v>
       </c>
@@ -1651,7 +1647,7 @@
         <f>IF(G7="LOW",200,100)*C7*10^(-9)/(I7*10^(-6))</f>
         <v>1.2727272727272727</v>
       </c>
-      <c r="AG7" s="33">
+      <c r="AG7" s="21">
         <f>T7/2</f>
         <v>0.79545454545454553</v>
       </c>
@@ -1693,10 +1689,10 @@
       <c r="L8" s="18">
         <v>22</v>
       </c>
-      <c r="M8" s="44">
+      <c r="M8" s="23">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="N8" s="37">
+      <c r="N8" s="22">
         <f>IF(G8="LOW",1.25,2.5)</f>
         <v>1.25</v>
       </c>
@@ -1772,13 +1768,28 @@
         <f>IF(G8="LOW",200,100)*C8*10^(-9)/(I8*10^(-6))</f>
         <v>1.2727272727272727</v>
       </c>
-      <c r="AG8" s="33">
+      <c r="AG8" s="21">
         <f>T8/2</f>
         <v>0.79545454545454553</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="AB1:AG1"/>
+    <mergeCell ref="AB2:AB3"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="AG2:AG3"/>
+    <mergeCell ref="Z2:AA2"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="B1:M1"/>
@@ -1789,70 +1800,55 @@
     <mergeCell ref="T2:T3"/>
     <mergeCell ref="U2:U3"/>
     <mergeCell ref="V2:V3"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="AB1:AG1"/>
-    <mergeCell ref="AB2:AB3"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="AG2:AG3"/>
-    <mergeCell ref="Z2:AA2"/>
     <mergeCell ref="R2:S2"/>
     <mergeCell ref="W2:W3"/>
     <mergeCell ref="X2:X3"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="Z4:Z8">
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="lessThan">
-      <formula>50</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U4:U8">
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="greaterThan">
-      <formula>2.8</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF4:AF8">
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="greaterThan">
-      <formula>2.8</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F4:F8">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B4:B8">
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="lessThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C8">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="greaterThan">
       <formula>17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D8">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F4:F8">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="greaterThan">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="Q4:Q8">
-    <cfRule type="cellIs" dxfId="0" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="12" operator="greaterThan">
       <formula>C4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U4:U8">
+    <cfRule type="cellIs" dxfId="2" priority="10" operator="greaterThan">
+      <formula>2.8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z4:Z8">
+    <cfRule type="cellIs" dxfId="1" priority="11" operator="lessThan">
+      <formula>50</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF4:AF8">
+    <cfRule type="cellIs" dxfId="0" priority="9" operator="greaterThan">
+      <formula>2.8</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -1869,7 +1865,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1879,7 +1875,7 @@
         <v>19</v>
       </c>
       <c r="B1">
-        <v>100</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
@@ -1887,7 +1883,7 @@
         <v>20</v>
       </c>
       <c r="B2">
-        <v>226</v>
+        <v>54.9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -1896,7 +1892,7 @@
       </c>
       <c r="B3">
         <f>(B1/B2+1)*0.7</f>
-        <v>1.0097345132743363</v>
+        <v>3.3138433515482699</v>
       </c>
     </row>
   </sheetData>

</xml_diff>